<commit_message>
Adding files containing info from original analysis
</commit_message>
<xml_diff>
--- a/results_from_original_2014_analysis/all_results.xlsx
+++ b/results_from_original_2014_analysis/all_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="1260" windowWidth="25360" windowHeight="15200" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="9420" yWindow="1260" windowWidth="25360" windowHeight="15200" tabRatio="500" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Q1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="650">
   <si>
     <t>Number</t>
   </si>
@@ -1921,9 +1921,6 @@
     <t>xmgrace</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Lecturer</t>
   </si>
   <si>
@@ -1966,9 +1963,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -1981,16 +1975,10 @@
     <t>No response</t>
   </si>
   <si>
-    <t>Contract</t>
-  </si>
-  <si>
     <t>Fixed term</t>
   </si>
   <si>
     <t>Permanent</t>
-  </si>
-  <si>
-    <t>OS</t>
   </si>
   <si>
     <t>Microsoft Windows</t>
@@ -7136,22 +7124,19 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>626</v>
-      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B2">
         <v>95</v>
@@ -7159,7 +7144,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B3">
         <v>75</v>
@@ -7167,7 +7152,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -7175,7 +7160,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -7183,7 +7168,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B6">
         <v>48</v>
@@ -7191,7 +7176,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B7">
         <v>19</v>
@@ -7199,7 +7184,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -7207,7 +7192,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B9">
         <v>51</v>
@@ -7215,7 +7200,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B10">
         <v>49</v>
@@ -7223,7 +7208,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -7231,7 +7216,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -7239,7 +7224,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -7247,7 +7232,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7255,7 +7240,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B15">
         <v>29</v>
@@ -7270,23 +7255,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>641</v>
-      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B2">
         <v>148</v>
@@ -7294,7 +7274,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B3">
         <v>257</v>
@@ -7302,7 +7282,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -7310,7 +7290,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -7318,7 +7298,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -7333,23 +7313,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>646</v>
-      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B2">
         <v>207</v>
@@ -7357,7 +7332,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B3">
         <v>184</v>
@@ -7365,7 +7340,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -7373,7 +7348,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -7388,23 +7363,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>649</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B2">
         <v>189</v>
@@ -7412,7 +7383,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B3">
         <v>99</v>
@@ -7420,7 +7391,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B4">
         <v>81</v>
@@ -7428,7 +7399,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B5">
         <v>41</v>
@@ -7436,7 +7407,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -7444,7 +7415,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -7511,7 +7482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>